<commit_message>
include rates for 2024
</commit_message>
<xml_diff>
--- a/examples/template.xlsx
+++ b/examples/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19453B75-4BE4-46A8-A6D1-75D0038F7200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E53E5-5B3C-4BD3-96D0-CEABA23466D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-28920" yWindow="12570" windowWidth="29040" windowHeight="15720" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Kim" sheetId="1" r:id="rId1"/>
@@ -429,27 +429,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="13" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -879,6 +869,11 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2056</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>2057</v>
       </c>
     </row>
   </sheetData>
@@ -892,20 +887,13 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="J1" sqref="J1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" customWidth="1"/>
+    <col min="2" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>